<commit_message>
Re-ran analysis.py on new synthetic volumes to correct angle calcs (they look good now)
</commit_message>
<xml_diff>
--- a/analysis/summary.xlsx
+++ b/analysis/summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brainlab-my.sharepoint.com/personal/shane_sicienski_snke_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\catalyst-tools\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{9D4FBB6E-B350-4A91-BCCB-4904B78EF070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31B64094-0158-4D21-8AFB-5D10570C9869}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6CB0D04-1D03-4898-ADE5-0C80CBCF1D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31960" yWindow="5380" windowWidth="28830" windowHeight="15830" xr2:uid="{DD260F35-B0C6-41E4-9255-0D5718BE7328}"/>
+    <workbookView xWindow="-37640" yWindow="3030" windowWidth="36750" windowHeight="19860" xr2:uid="{DD260F35-B0C6-41E4-9255-0D5718BE7328}"/>
   </bookViews>
   <sheets>
     <sheet name="SegThy" sheetId="1" r:id="rId1"/>
@@ -412,7 +412,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -912,7 +912,7 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -977,10 +977,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1303,7 +1299,7 @@
   <dimension ref="A1:AC33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AD9" sqref="AD9"/>
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.75"/>
@@ -4151,8 +4147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64BC1F98-15C7-469E-BB0C-F6C580CA5A51}">
   <dimension ref="A1:AC17"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA21" sqref="AA21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.75"/>
@@ -4322,16 +4318,16 @@
         <v>7.9781572820762898</v>
       </c>
       <c r="T2" s="2">
-        <v>-147.55505117097999</v>
+        <v>-112.483254668527</v>
       </c>
       <c r="U2" s="2">
-        <v>131.201048872233</v>
+        <v>32.444948829019403</v>
       </c>
       <c r="V2" s="2">
-        <v>83.033481929329099</v>
+        <v>-92.680803784956595</v>
       </c>
       <c r="W2" s="2">
-        <v>31.4457111312317</v>
+        <v>23.170010867658998</v>
       </c>
       <c r="X2" s="2">
         <v>3.2683982879230098</v>
@@ -4408,16 +4404,16 @@
         <v>16.507353616791502</v>
       </c>
       <c r="T3" s="2">
-        <v>-114.07918656408999</v>
+        <v>-74.9592337686245</v>
       </c>
       <c r="U3" s="2">
-        <v>163.14846759516001</v>
+        <v>65.920813435909295</v>
       </c>
       <c r="V3" s="2">
-        <v>119.241661137145</v>
+        <v>-56.083014187529599</v>
       </c>
       <c r="W3" s="2">
-        <v>32.1518018272888</v>
+        <v>22.656017964062301</v>
       </c>
       <c r="X3" s="2">
         <v>3.5662640255398599</v>
@@ -4494,16 +4490,16 @@
         <v>16.481664809247</v>
       </c>
       <c r="T4" s="2">
-        <v>-179.914086594119</v>
+        <v>-22.515745623197699</v>
       </c>
       <c r="U4" s="2">
-        <v>179.07539909174</v>
+        <v>50.076068502654699</v>
       </c>
       <c r="V4" s="2">
-        <v>58.954084172726802</v>
+        <v>-5.66130044265776</v>
       </c>
       <c r="W4" s="2">
-        <v>152.80369783482499</v>
+        <v>17.727140255431401</v>
       </c>
       <c r="X4" s="2">
         <v>3.8498339034951501</v>
@@ -4580,16 +4576,16 @@
         <v>10.3136418521603</v>
       </c>
       <c r="T5" s="2">
-        <v>-142.243113763786</v>
+        <v>-106.688249581566</v>
       </c>
       <c r="U5" s="2">
-        <v>123.963989333478</v>
+        <v>41.573561062288903</v>
       </c>
       <c r="V5" s="2">
-        <v>85.446771294860099</v>
+        <v>-85.981800133711204</v>
       </c>
       <c r="W5" s="2">
-        <v>39.539612609171201</v>
+        <v>26.553437563913501</v>
       </c>
       <c r="X5" s="2">
         <v>2.5484461878787399</v>
@@ -4666,16 +4662,16 @@
         <v>10.1601834890362</v>
       </c>
       <c r="T6" s="2">
-        <v>-169.35976235779799</v>
+        <v>-66.088725975100999</v>
       </c>
       <c r="U6" s="2">
-        <v>176.37047136095799</v>
+        <v>10.640237642201299</v>
       </c>
       <c r="V6" s="2">
-        <v>126.85505158824201</v>
+        <v>-48.469623736432503</v>
       </c>
       <c r="W6" s="2">
-        <v>38.221775167142802</v>
+        <v>18.771293550193299</v>
       </c>
       <c r="X6" s="2">
         <v>2.6373713747497698</v>
@@ -4752,16 +4748,16 @@
         <v>10.7938622735532</v>
       </c>
       <c r="T7" s="2">
-        <v>-178.86728957225</v>
+        <v>-31.2275811003014</v>
       </c>
       <c r="U7" s="2">
-        <v>178.95617502333999</v>
+        <v>37.498054018220699</v>
       </c>
       <c r="V7" s="2">
-        <v>78.314110691935099</v>
+        <v>-12.854720476895899</v>
       </c>
       <c r="W7" s="2">
-        <v>137.908800800688</v>
+        <v>20.0117022595701</v>
       </c>
       <c r="X7" s="2">
         <v>2.8091981706973401</v>
@@ -4838,16 +4834,16 @@
         <v>10.4899275723402</v>
       </c>
       <c r="T8" s="2">
-        <v>-37.754387700046799</v>
+        <v>-178.989102095037</v>
       </c>
       <c r="U8" s="2">
-        <v>36.758922423373598</v>
+        <v>178.79866144223899</v>
       </c>
       <c r="V8" s="2">
-        <v>-5.6760679784512504</v>
+        <v>18.1793537082957</v>
       </c>
       <c r="W8" s="2">
-        <v>24.019695934329501</v>
+        <v>157.434413673243</v>
       </c>
       <c r="X8" s="2">
         <v>3.0707777503426601</v>
@@ -4924,16 +4920,16 @@
         <v>4.8664327532728802</v>
       </c>
       <c r="T9" s="2">
-        <v>-56.956163547834898</v>
+        <v>-173.81513626117999</v>
       </c>
       <c r="U9" s="2">
-        <v>109.37908122005</v>
+        <v>170.07074452297499</v>
       </c>
       <c r="V9" s="2">
-        <v>70.343579819076496</v>
+        <v>-100.65642018092301</v>
       </c>
       <c r="W9" s="2">
-        <v>25.563738181860099</v>
+        <v>44.094801302008101</v>
       </c>
       <c r="X9" s="2">
         <v>1.78195512953193</v>
@@ -5010,13 +5006,13 @@
         <v>4.2224486474316301</v>
       </c>
       <c r="T10" s="2">
-        <v>54.071015308008903</v>
+        <v>-125.928984691991</v>
       </c>
       <c r="U10" s="2">
-        <v>152.765375069085</v>
+        <v>-27.234624930914698</v>
       </c>
       <c r="V10" s="2">
-        <v>116.92030604458699</v>
+        <v>-63.0796939554129</v>
       </c>
       <c r="W10" s="2">
         <v>19.037821035642899</v>
@@ -5096,16 +5092,16 @@
         <v>4.0839815998036801</v>
       </c>
       <c r="T11" s="2">
-        <v>-179.556758683997</v>
+        <v>-28.738070977922</v>
       </c>
       <c r="U11" s="2">
-        <v>177.36863331187101</v>
+        <v>44.800276363492699</v>
       </c>
       <c r="V11" s="2">
-        <v>80.298140427478202</v>
+        <v>-10.8129706836328</v>
       </c>
       <c r="W11" s="2">
-        <v>136.457507326925</v>
+        <v>20.822539013200601</v>
       </c>
       <c r="X11" s="2">
         <v>2.0514918038341499</v>
@@ -5182,13 +5178,13 @@
         <v>15.192095999286501</v>
       </c>
       <c r="T12" s="2">
-        <v>59.144524015414802</v>
+        <v>-120.855475984585</v>
       </c>
       <c r="U12" s="2">
-        <v>125.77740044226699</v>
+        <v>-54.222599557732799</v>
       </c>
       <c r="V12" s="2">
-        <v>79.604055849555195</v>
+        <v>-100.395944150444</v>
       </c>
       <c r="W12" s="2">
         <v>23.371622855112498</v>
@@ -5268,16 +5264,16 @@
         <v>14.8832262637283</v>
       </c>
       <c r="T13" s="2">
-        <v>-176.46341337768101</v>
+        <v>-73.315389667923398</v>
       </c>
       <c r="U13" s="2">
-        <v>179.70737404955401</v>
+        <v>73.617851897805593</v>
       </c>
       <c r="V13" s="2">
-        <v>115.996461708189</v>
+        <v>-49.977564265835902</v>
       </c>
       <c r="W13" s="2">
-        <v>57.146785899313898</v>
+        <v>28.377580218663699</v>
       </c>
       <c r="X13" s="2">
         <v>4.5866144200827303</v>
@@ -5354,16 +5350,16 @@
         <v>15.544939146087399</v>
       </c>
       <c r="T14" s="2">
-        <v>-179.575760533123</v>
+        <v>-18.835588482217702</v>
       </c>
       <c r="U14" s="2">
-        <v>179.417073889954</v>
+        <v>53.382182517231499</v>
       </c>
       <c r="V14" s="2">
-        <v>52.284013140960397</v>
+        <v>-3.1006022436549601</v>
       </c>
       <c r="W14" s="2">
-        <v>156.45945618952101</v>
+        <v>17.2440059382077</v>
       </c>
       <c r="X14" s="2">
         <v>5.2970740398205303</v>
@@ -5440,13 +5436,13 @@
         <v>3.0063902166149901</v>
       </c>
       <c r="T15" s="2">
-        <v>62.230087765609497</v>
+        <v>-117.76991223439001</v>
       </c>
       <c r="U15" s="2">
-        <v>124.05245765567599</v>
+        <v>-55.947542344323601</v>
       </c>
       <c r="V15" s="2">
-        <v>83.755466040201597</v>
+        <v>-96.244533959798304</v>
       </c>
       <c r="W15" s="2">
         <v>19.2843210403962</v>
@@ -5526,16 +5522,16 @@
         <v>2.9304499103771202</v>
       </c>
       <c r="T16" s="2">
-        <v>-178.522422757638</v>
+        <v>-84.521341266425196</v>
       </c>
       <c r="U16" s="2">
-        <v>178.80787495421799</v>
+        <v>94.827562968532305</v>
       </c>
       <c r="V16" s="2">
-        <v>106.418169936395</v>
+        <v>-50.5049069866811</v>
       </c>
       <c r="W16" s="2">
-        <v>69.6974897144473</v>
+        <v>37.8906191589803</v>
       </c>
       <c r="X16" s="2">
         <v>0.90726269809174598</v>
@@ -5612,16 +5608,16 @@
         <v>3.3644349603568302</v>
       </c>
       <c r="T17" s="2">
-        <v>-178.888989925554</v>
+        <v>-39.136416276149397</v>
       </c>
       <c r="U17" s="2">
-        <v>179.62972810774701</v>
+        <v>52.599191885376499</v>
       </c>
       <c r="V17" s="2">
-        <v>68.239211078882605</v>
+        <v>-12.287104710591001</v>
       </c>
       <c r="W17" s="2">
-        <v>137.58667135791899</v>
+        <v>27.399408084431901</v>
       </c>
       <c r="X17" s="2">
         <v>0.81483819590774198</v>

</xml_diff>